<commit_message>
so this cannot be empty?
</commit_message>
<xml_diff>
--- a/controller_board/Analog_board_BOM.xlsx
+++ b/controller_board/Analog_board_BOM.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors" sheetId="1" r:id="rId1"/>
     <sheet name="Capacitors" sheetId="2" r:id="rId2"/>
+    <sheet name="By the numbers" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="273">
   <si>
     <t>Name</t>
   </si>
@@ -630,21 +631,9 @@
     <t>&lt;mW</t>
   </si>
   <si>
-    <t>1k5</t>
-  </si>
-  <si>
-    <t>20 mW</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/8029933/</t>
-  </si>
-  <si>
-    <t>680n</t>
-  </si>
-  <si>
     <t>43k2</t>
   </si>
   <si>
@@ -657,24 +646,9 @@
     <t>83 mW</t>
   </si>
   <si>
-    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/6480957/</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>33k2</t>
-  </si>
-  <si>
-    <t>16k5</t>
-  </si>
-  <si>
-    <t>14k</t>
-  </si>
-  <si>
     <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/8029860/</t>
   </si>
   <si>
@@ -693,44 +667,191 @@
     <t>&lt;uW</t>
   </si>
   <si>
-    <t>5k</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/6984119/</t>
-  </si>
-  <si>
-    <t>82p</t>
-  </si>
-  <si>
-    <t>2k5</t>
-  </si>
-  <si>
-    <t>60k4</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>4k75</t>
-  </si>
-  <si>
-    <t>23k7</t>
-  </si>
-  <si>
     <t>7k5</t>
   </si>
   <si>
     <t>4k48</t>
+  </si>
+  <si>
+    <t>12k4</t>
+  </si>
+  <si>
+    <t>12mW</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/7236262/</t>
+  </si>
+  <si>
+    <t>270p</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>4k02</t>
+  </si>
+  <si>
+    <t>95k3</t>
+  </si>
+  <si>
+    <t>768</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Decoupling</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>R03,R04</t>
+  </si>
+  <si>
+    <t>R33,R34,R35</t>
+  </si>
+  <si>
+    <t>R37,R42</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>R08,R12,R19,R22,R24,R29</t>
+  </si>
+  <si>
+    <t>R13,R17,R30</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>R18,R23,R31</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voltage </t>
+  </si>
+  <si>
+    <t>330n</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/6983557/</t>
+  </si>
+  <si>
+    <t>C03,C04,C05</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>C01,C02</t>
+  </si>
+  <si>
+    <t>in stock</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7215666/</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>681</t>
+  </si>
+  <si>
+    <t>R05, R06, R07, R09, R10, R11, R14, R15, R16, R20, R21, R25, R27, R28, R32, R39, R43, R44, R45, R46, R47, R48</t>
+  </si>
+  <si>
+    <t>3k57</t>
+  </si>
+  <si>
+    <t>90k9</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086089/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086297/</t>
+  </si>
+  <si>
+    <t>4k42</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086326/</t>
+  </si>
+  <si>
+    <t>package quantity</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086345/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/6662588/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086436/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/6790863/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086470/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/8326741/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086610/</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/overflademontering-faste-modstande/7086711/</t>
+  </si>
+  <si>
+    <t>C06, C08, C15, C17, C19, C21, C23, C25, C27, C29, C31, C33</t>
+  </si>
+  <si>
+    <t>C07, C09, C16, C18, C20, C22, C24, C26, C28, C30, C32, C34</t>
+  </si>
+  <si>
+    <t>http://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/6983421/</t>
+  </si>
+  <si>
+    <t>Boards</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>Quantity per Board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,25 +859,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -768,17 +877,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1057,13 +1166,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H116"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11940" ySplit="576" topLeftCell="M16" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="11940" ySplit="576" topLeftCell="M25" activePane="bottomLeft"/>
       <selection sqref="A1:E1048576"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -1095,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>121</v>
@@ -1104,7 +1213,7 @@
         <v>196</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1112,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>121</v>
@@ -1121,7 +1230,7 @@
         <v>196</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,7 +1247,7 @@
         <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1155,7 +1264,7 @@
         <v>196</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1214,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>121</v>
@@ -1228,7 +1337,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>121</v>
@@ -1242,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>121</v>
@@ -1256,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>121</v>
@@ -1270,7 +1379,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>121</v>
@@ -1284,7 +1393,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>121</v>
@@ -1312,7 +1421,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>121</v>
@@ -1326,7 +1435,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>121</v>
@@ -1340,7 +1449,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>121</v>
@@ -1354,7 +1463,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>121</v>
@@ -1368,7 +1477,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>121</v>
@@ -1382,7 +1491,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>121</v>
@@ -1410,7 +1519,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>121</v>
@@ -1424,7 +1533,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>121</v>
@@ -1438,7 +1547,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>121</v>
@@ -1465,17 +1574,17 @@
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>202</v>
+      <c r="B27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
@@ -1485,7 +1594,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>121</v>
@@ -1499,7 +1608,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>121</v>
@@ -1513,7 +1622,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>121</v>
@@ -1527,7 +1636,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>121</v>
@@ -1541,7 +1650,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>121</v>
@@ -1550,12 +1659,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>197</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>121</v>
@@ -1564,12 +1673,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>121</v>
@@ -1578,12 +1687,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>121</v>
@@ -1592,12 +1701,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>121</v>
@@ -1606,12 +1715,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>121</v>
@@ -1620,12 +1729,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>121</v>
@@ -1633,13 +1742,16 @@
       <c r="D38" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>121</v>
@@ -1648,7 +1760,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1665,12 +1777,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>121</v>
@@ -1682,12 +1794,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>121</v>
@@ -1699,12 +1811,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>121</v>
@@ -1716,12 +1828,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>121</v>
@@ -1730,15 +1842,15 @@
         <v>196</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>121</v>
@@ -1746,16 +1858,13 @@
       <c r="D45" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>121</v>
@@ -1763,96 +1872,120 @@
       <c r="D46" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -2127,7 +2260,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A11" sqref="A11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,7 +2288,7 @@
         <v>125</v>
       </c>
       <c r="G1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2163,7 +2296,7 @@
         <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>121</v>
@@ -2172,13 +2305,13 @@
         <v>196</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2186,7 +2319,7 @@
         <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
@@ -2195,13 +2328,13 @@
         <v>196</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2209,7 +2342,7 @@
         <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
         <v>121</v>
@@ -2218,13 +2351,13 @@
         <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G4" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2232,7 +2365,7 @@
         <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
         <v>121</v>
@@ -2241,13 +2374,13 @@
         <v>196</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2255,7 +2388,7 @@
         <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>121</v>
@@ -2264,41 +2397,113 @@
         <v>196</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>131</v>
       </c>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G7" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>132</v>
       </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G8" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>133</v>
       </c>
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G9" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>134</v>
       </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>121</v>
@@ -2313,31 +2518,13 @@
         <v>195</v>
       </c>
       <c r="G11" t="s">
-        <v>204</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>136</v>
       </c>
-      <c r="B12" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F12" t="s">
-        <v>195</v>
-      </c>
-      <c r="G12" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2358,163 +2545,535 @@
       <c r="A16" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" t="s">
+        <v>210</v>
+      </c>
+      <c r="G17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F19" t="s">
+        <v>210</v>
+      </c>
+      <c r="G19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F22" t="s">
+        <v>210</v>
+      </c>
+      <c r="G22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F23" t="s">
+        <v>210</v>
+      </c>
+      <c r="G23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" t="s">
+        <v>210</v>
+      </c>
+      <c r="G24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F25" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F27" t="s">
+        <v>210</v>
+      </c>
+      <c r="G27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F28" t="s">
+        <v>210</v>
+      </c>
+      <c r="G28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F29" t="s">
+        <v>210</v>
+      </c>
+      <c r="G29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" t="s">
+        <v>210</v>
+      </c>
+      <c r="G30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F31" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F32" t="s">
+        <v>210</v>
+      </c>
+      <c r="G32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" t="s">
+        <v>210</v>
+      </c>
+      <c r="G33" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F34" t="s">
+        <v>210</v>
+      </c>
+      <c r="G34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F35" t="s">
+        <v>210</v>
+      </c>
+      <c r="G35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>172</v>
       </c>
@@ -2632,4 +3191,596 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+      <c r="P1" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" t="s">
+        <v>247</v>
+      </c>
+      <c r="P2" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q2">
+        <f>SUM(H3:H23)</f>
+        <v>112.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>B3*$Q$1</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3">
+        <v>1.478</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <f>ROUNDUP(C3/G3,0)*(F3*G3)</f>
+        <v>7.39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C15" si="0">B4*$Q$1</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F4">
+        <v>2.6139999999999999</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H23" si="1">ROUNDUP(C4/G4,0)*(F4*G4)</f>
+        <v>13.07</v>
+      </c>
+      <c r="I4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F5">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.6300000000000001</v>
+      </c>
+      <c r="I5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1.976</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>9.879999999999999</v>
+      </c>
+      <c r="I6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7">
+        <v>1.976</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>9.879999999999999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>3.27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.6300000000000001</v>
+      </c>
+      <c r="I10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>0.08</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>1.976</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>9.879999999999999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="I13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1.7100000000000002</v>
+      </c>
+      <c r="I14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15">
+        <v>2.1</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C23" si="2">B18*$Q$1</f>
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>30.2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D21" s="1">
+        <v>15</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I21" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>6.5500000000000007</v>
+      </c>
+      <c r="I23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:G49">
+    <sortCondition ref="B1:B49"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>